<commit_message>
Updated the Template to be easier to use
</commit_message>
<xml_diff>
--- a/Git Hub Data Excel/Feb_2008.xlsx
+++ b/Git Hub Data Excel/Feb_2008.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\seng403_New\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\seng403_New\Git Hub Data Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Tabulation Manipulation Page" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Formatted Data'!$J$2:$J$29</definedName>
     <definedName name="Feb_2008" localSheetId="1">RAW!$A$1:$C$188</definedName>
     <definedName name="Feb_2008_LOC" localSheetId="1">RAW!$I$1:$L$50</definedName>
     <definedName name="Feb_2008_LOC" localSheetId="2">'Tabulation Manipulation Page'!$G$1:$J$50</definedName>
@@ -30,6 +29,41 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>User</author>
+  </authors>
+  <commentList>
+    <comment ref="L2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Corresponds to list of components
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
@@ -77,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="83">
   <si>
     <t>GHTorrentName</t>
   </si>
@@ -318,12 +352,21 @@
   <si>
     <t>Elliot Horowitz</t>
   </si>
+  <si>
+    <t>Dwight Ownership</t>
+  </si>
+  <si>
+    <t>Elliot Horowitz Ownership</t>
+  </si>
+  <si>
+    <t>yellow Ownership</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +386,19 @@
       <color rgb="FF0A0101"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -372,13 +428,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,15 +455,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Feb_2008_LOC" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Feb_2008" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Feb_2008" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Feb_2008_LOC_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Feb_2008_LOC_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Feb_2008_LOC" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -675,11 +732,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1282"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U1282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,18 +747,18 @@
     <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="24" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" customWidth="1"/>
+    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,7 +777,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -734,26 +791,35 @@
         <v>15</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="2"/>
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>17</v>
@@ -766,23 +832,56 @@
       <c r="F2" s="1">
         <v>2</v>
       </c>
+      <c r="G2" s="4">
+        <f>L2</f>
+        <v>1</v>
+      </c>
       <c r="H2" s="1">
         <v>0</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="1" t="str">
-        <f>IF(D2="","",IF(COUNTIF($D2:D183,D2)=1,D2,""))</f>
-        <v/>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <f>IF(D97="","",IF(COUNTIF($D97:D283,D97)=1,D97,""))</f>
+        <v>grid/</v>
+      </c>
+      <c r="K2" s="1">
+        <f>SUMPRODUCT(SUMIF($D$1:$D$183,J2,$H$1:$H$183))</f>
+        <v>17.041999999999998</v>
+      </c>
+      <c r="L2" s="4">
+        <f>SUMPRODUCT(SUMIF($D$1:$D$133,J2,$H$1:$H$133))/K2</f>
+        <v>1</v>
+      </c>
+      <c r="M2" s="6">
+        <f>G135</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <f>G158</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="6">
+        <f>MAX(L2:N2)</f>
+        <v>1</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="1">
+        <v>3</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -795,28 +894,57 @@
       <c r="F3" s="1">
         <v>2</v>
       </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G5" si="0">L3</f>
+        <v>0.97124636728658131</v>
+      </c>
       <c r="H3" s="1">
         <f>F3*E3</f>
         <v>2</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="1" t="str">
-        <f>IF(D97="","",IF(COUNTIF($D97:D283,D97)=1,D97,""))</f>
-        <v>grid/</v>
+        <f>IF(D157="","",IF(COUNTIF($D157:D343,D157)=1,D157,""))</f>
+        <v>db/</v>
       </c>
       <c r="K3" s="1">
-        <f ca="1">SUMPRODUCT(SUMIF($D$1:$D$183,J3,$H$1:$H$83))</f>
-        <v>17.041999999999998</v>
-      </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <f>SUMPRODUCT(SUMIF($D$1:$D$183,J3,$H$1:$H$183))</f>
+        <v>486.89499999999992</v>
+      </c>
+      <c r="L3" s="4">
+        <f>SUMPRODUCT(SUMIF($D$1:$D$133,J3,$H$1:$H$133))/K3</f>
+        <v>0.97124636728658131</v>
+      </c>
+      <c r="M3" s="6">
+        <f t="shared" ref="M3:M5" si="1">G136</f>
+        <v>2.8753632713418707E-2</v>
+      </c>
+      <c r="N3" s="6">
+        <f t="shared" ref="N3:N5" si="2">G159</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6">
+        <f t="shared" ref="Q3:Q5" si="3">MAX(L3:N3)</f>
+        <v>0.97124636728658131</v>
+      </c>
+      <c r="R3" s="2"/>
+      <c r="S3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -827,28 +955,57 @@
       <c r="F4" s="1">
         <v>13</v>
       </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H4" s="1" t="str">
         <f>IF($E4*$F4=0,"",$E4*$F4)</f>
         <v/>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="1" t="str">
-        <f>IF(D157="","",IF(COUNTIF($D157:D343,D157)=1,D157,""))</f>
-        <v>db/</v>
+        <f>IF(D179="","",IF(COUNTIF($D179:D365,D179)=1,D179,""))</f>
+        <v>bin/</v>
       </c>
       <c r="K4" s="1">
-        <f ca="1">SUMPRODUCT(SUMIF($D$1:$D$183,J4,$H$1:$H$83))</f>
-        <v>486.89499999999992</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <f>SUMPRODUCT(SUMIF($D$1:$D$183,J4,$H$1:$H$183))</f>
+        <v>15</v>
+      </c>
+      <c r="L4" s="4">
+        <f>SUMPRODUCT(SUMIF($D$1:$D$133,J4,$H$1:$H$133))/K4</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="T4" s="1">
+        <v>2</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -861,28 +1018,51 @@
       <c r="F5" s="1">
         <v>13</v>
       </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>7.1911861565175733E-2</v>
+      </c>
       <c r="H5" s="1">
         <f>IF($E5*$F5=0,"",$E5*$F5)</f>
         <v>13</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="1" t="str">
-        <f>IF(D179="","",IF(COUNTIF($D179:D365,D179)=1,D179,""))</f>
-        <v>bin/</v>
+        <f>IF(D183="","",IF(COUNTIF($D183:D369,D183)=1,D183,""))</f>
+        <v>util/</v>
       </c>
       <c r="K5" s="1">
-        <f ca="1">SUMPRODUCT(SUMIF($D$1:$D$183,J5,$H$1:$H$83))</f>
-        <v>15</v>
-      </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <f>SUMPRODUCT(SUMIF($D$1:$D$183,J5,$H$1:$H$183))</f>
+        <v>33.402000000000001</v>
+      </c>
+      <c r="L5" s="4">
+        <f>SUMPRODUCT(SUMIF($D$1:$D$133,J5,$H$1:$H$133))/K5</f>
+        <v>7.1911861565175733E-2</v>
+      </c>
+      <c r="M5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.11975330818513862</v>
+      </c>
+      <c r="N5" s="6">
+        <f t="shared" si="2"/>
+        <v>0.80833483024968567</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="6">
+        <f t="shared" si="3"/>
+        <v>0.80833483024968567</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -893,31 +1073,24 @@
       <c r="F6" s="1">
         <v>37</v>
       </c>
-      <c r="G6" s="1">
-        <v>-1</v>
-      </c>
       <c r="H6" s="1" t="str">
-        <f t="shared" ref="H4:H64" si="0">IF($E6*$F6=0,"",$E6*$F6)</f>
+        <f t="shared" ref="H6:H64" si="4">IF($E6*$F6=0,"",$E6*$F6)</f>
         <v/>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="1" t="str">
-        <f>IF(D183="","",IF(COUNTIF($D183:D369,D183)=1,D183,""))</f>
-        <v>util/</v>
-      </c>
-      <c r="K6" s="1">
-        <f ca="1">SUMPRODUCT(SUMIF($D$1:$D$183,J6,$H$1:$H$83))</f>
-        <v>33.402000000000001</v>
-      </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="2"/>
+        <f>IF(D184="","",IF(COUNTIF($D184:D370,D184)=1,D184,""))</f>
+        <v/>
+      </c>
+      <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="2"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -931,23 +1104,23 @@
         <v>37</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="1" t="str">
-        <f>IF(D184="","",IF(COUNTIF($D184:D370,D184)=1,D184,""))</f>
-        <v/>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="2"/>
+        <f>IF(D185="","",IF(COUNTIF($D185:D371,D185)=1,D185,""))</f>
+        <v/>
+      </c>
+      <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R7" s="2"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -957,23 +1130,23 @@
         <v>37</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="1" t="str">
-        <f>IF(D185="","",IF(COUNTIF($D185:D371,D185)=1,D185,""))</f>
-        <v/>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="2"/>
+        <f>IF(D186="","",IF(COUNTIF($D186:D372,D186)=1,D186,""))</f>
+        <v/>
+      </c>
+      <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R8" s="2"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -985,23 +1158,23 @@
         <v>26</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="1" t="str">
-        <f>IF(D186="","",IF(COUNTIF($D186:D372,D186)=1,D186,""))</f>
-        <v/>
-      </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="2"/>
+        <f>IF(D187="","",IF(COUNTIF($D187:D373,D187)=1,D187,""))</f>
+        <v/>
+      </c>
+      <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R9" s="2"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1011,23 +1184,23 @@
         <v>26</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="1" t="str">
-        <f>IF(D187="","",IF(COUNTIF($D187:D373,D187)=1,D187,""))</f>
-        <v/>
-      </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="2"/>
+        <f>IF(D188="","",IF(COUNTIF($D188:D374,D188)=1,D188,""))</f>
+        <v/>
+      </c>
+      <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="2"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1041,46 +1214,46 @@
         <v>26</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="1" t="str">
-        <f>IF(D188="","",IF(COUNTIF($D188:D374,D188)=1,D188,""))</f>
-        <v/>
-      </c>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="2"/>
+        <f>IF(D189="","",IF(COUNTIF($D189:D375,D189)=1,D189,""))</f>
+        <v/>
+      </c>
+      <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R11" s="2"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
       <c r="F12" s="1">
         <v>26</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="1" t="str">
-        <f>IF(D189="","",IF(COUNTIF($D189:D375,D189)=1,D189,""))</f>
-        <v/>
-      </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="2"/>
+        <f>IF(D190="","",IF(COUNTIF($D190:D376,D190)=1,D190,""))</f>
+        <v/>
+      </c>
+      <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R12" s="2"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>23</v>
       </c>
@@ -1090,46 +1263,46 @@
         <v>9</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="1" t="str">
-        <f>IF(D190="","",IF(COUNTIF($D190:D376,D190)=1,D190,""))</f>
-        <v/>
-      </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="2"/>
+        <f>IF(D191="","",IF(COUNTIF($D191:D377,D191)=1,D191,""))</f>
+        <v/>
+      </c>
+      <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R13" s="2"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="E14" s="4"/>
       <c r="F14" s="1">
         <v>9</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="1" t="str">
-        <f>IF(D191="","",IF(COUNTIF($D191:D377,D191)=1,D191,""))</f>
-        <v/>
-      </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="2"/>
+        <f>IF(D192="","",IF(COUNTIF($D192:D378,D192)=1,D192,""))</f>
+        <v/>
+      </c>
+      <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R14" s="2"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1140,46 +1313,46 @@
         <v>9</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="1" t="str">
-        <f>IF(D192="","",IF(COUNTIF($D192:D378,D192)=1,D192,""))</f>
-        <v/>
-      </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="2"/>
+        <f>IF(D193="","",IF(COUNTIF($D193:D379,D193)=1,D193,""))</f>
+        <v/>
+      </c>
+      <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R15" s="2"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="E16" s="4"/>
       <c r="F16" s="1">
         <v>9</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="1" t="str">
-        <f>IF(D193="","",IF(COUNTIF($D193:D379,D193)=1,D193,""))</f>
-        <v/>
-      </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="2"/>
+        <f>IF(D194="","",IF(COUNTIF($D194:D380,D194)=1,D194,""))</f>
+        <v/>
+      </c>
+      <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R16" s="2"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>24</v>
       </c>
@@ -1189,40 +1362,40 @@
         <v>71</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="1" t="str">
-        <f>IF(D194="","",IF(COUNTIF($D194:D380,D194)=1,D194,""))</f>
-        <v/>
-      </c>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D195="","",IF(COUNTIF($D195:D381,D195)=1,D195,""))</f>
+        <v/>
+      </c>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="4"/>
       <c r="F18" s="1">
         <v>71</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="1" t="str">
-        <f>IF(D195="","",IF(COUNTIF($D195:D381,D195)=1,D195,""))</f>
-        <v/>
-      </c>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D196="","",IF(COUNTIF($D196:D382,D196)=1,D196,""))</f>
+        <v/>
+      </c>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1233,40 +1406,40 @@
         <v>71</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="1" t="str">
-        <f>IF(D196="","",IF(COUNTIF($D196:D382,D196)=1,D196,""))</f>
-        <v/>
-      </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="2"/>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D197="","",IF(COUNTIF($D197:D383,D197)=1,D197,""))</f>
+        <v/>
+      </c>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="4"/>
       <c r="F20" s="1">
         <v>71</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="1" t="str">
-        <f>IF(D197="","",IF(COUNTIF($D197:D383,D197)=1,D197,""))</f>
-        <v/>
-      </c>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D198="","",IF(COUNTIF($D198:D384,D198)=1,D198,""))</f>
+        <v/>
+      </c>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="2"/>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>25</v>
       </c>
@@ -1276,40 +1449,40 @@
         <v>16</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="1" t="str">
-        <f>IF(D198="","",IF(COUNTIF($D198:D384,D198)=1,D198,""))</f>
-        <v/>
-      </c>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D199="","",IF(COUNTIF($D199:D385,D199)=1,D199,""))</f>
+        <v/>
+      </c>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="2"/>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="E22" s="4"/>
       <c r="F22" s="1">
         <v>16</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="1" t="str">
-        <f>IF(D199="","",IF(COUNTIF($D199:D385,D199)=1,D199,""))</f>
-        <v/>
-      </c>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="2"/>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D200="","",IF(COUNTIF($D200:D386,D200)=1,D200,""))</f>
+        <v/>
+      </c>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1320,40 +1493,40 @@
         <v>16</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="1" t="str">
-        <f>IF(D200="","",IF(COUNTIF($D200:D386,D200)=1,D200,""))</f>
-        <v/>
-      </c>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="2"/>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D201="","",IF(COUNTIF($D201:D387,D201)=1,D201,""))</f>
+        <v/>
+      </c>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="E24" s="4"/>
       <c r="F24" s="1">
         <v>16</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="1" t="str">
-        <f>IF(D201="","",IF(COUNTIF($D201:D387,D201)=1,D201,""))</f>
-        <v/>
-      </c>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="2"/>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D202="","",IF(COUNTIF($D202:D388,D202)=1,D202,""))</f>
+        <v/>
+      </c>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>26</v>
       </c>
@@ -1363,40 +1536,40 @@
         <v>2</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="1" t="str">
-        <f>IF(D202="","",IF(COUNTIF($D202:D388,D202)=1,D202,""))</f>
-        <v/>
-      </c>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="2"/>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D203="","",IF(COUNTIF($D203:D389,D203)=1,D203,""))</f>
+        <v/>
+      </c>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="4"/>
       <c r="F26" s="1">
         <v>2</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="1" t="str">
-        <f>IF(D203="","",IF(COUNTIF($D203:D389,D203)=1,D203,""))</f>
-        <v/>
-      </c>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="2"/>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D204="","",IF(COUNTIF($D204:D390,D204)=1,D204,""))</f>
+        <v/>
+      </c>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="s">
         <v>19</v>
       </c>
@@ -1407,40 +1580,40 @@
         <v>2</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="1" t="str">
-        <f>IF(D204="","",IF(COUNTIF($D204:D390,D204)=1,D204,""))</f>
-        <v/>
-      </c>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="2"/>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D205="","",IF(COUNTIF($D205:D391,D205)=1,D205,""))</f>
+        <v/>
+      </c>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="4"/>
       <c r="F28" s="1">
         <v>2</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="1" t="str">
-        <f>IF(D205="","",IF(COUNTIF($D205:D391,D205)=1,D205,""))</f>
-        <v/>
-      </c>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="2"/>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D206="","",IF(COUNTIF($D206:D392,D206)=1,D206,""))</f>
+        <v/>
+      </c>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="2"/>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>27</v>
       </c>
@@ -1450,40 +1623,40 @@
         <v>1</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="1" t="str">
-        <f>IF(D206="","",IF(COUNTIF($D206:D392,D206)=1,D206,""))</f>
-        <v/>
-      </c>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="2"/>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D207="","",IF(COUNTIF($D207:D393,D207)=1,D207,""))</f>
+        <v/>
+      </c>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="2"/>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="4"/>
       <c r="F30" s="1">
         <v>1</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="1" t="str">
-        <f>IF(D207="","",IF(COUNTIF($D207:D393,D207)=1,D207,""))</f>
-        <v/>
-      </c>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="2"/>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D208="","",IF(COUNTIF($D208:D394,D208)=1,D208,""))</f>
+        <v/>
+      </c>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="2"/>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D31" s="1" t="s">
         <v>19</v>
       </c>
@@ -1494,40 +1667,40 @@
         <v>1</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="1" t="str">
-        <f>IF(D208="","",IF(COUNTIF($D208:D394,D208)=1,D208,""))</f>
-        <v/>
-      </c>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="2"/>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D209="","",IF(COUNTIF($D209:D395,D209)=1,D209,""))</f>
+        <v/>
+      </c>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="2"/>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="E32" s="4"/>
       <c r="F32" s="1">
         <v>1</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="1" t="str">
-        <f>IF(D209="","",IF(COUNTIF($D209:D395,D209)=1,D209,""))</f>
-        <v/>
-      </c>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="2"/>
-    </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D210="","",IF(COUNTIF($D210:D396,D210)=1,D210,""))</f>
+        <v/>
+      </c>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="2"/>
+    </row>
+    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>28</v>
       </c>
@@ -1537,40 +1710,40 @@
         <v>2</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="1" t="str">
-        <f>IF(D210="","",IF(COUNTIF($D210:D396,D210)=1,D210,""))</f>
-        <v/>
-      </c>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="2"/>
-    </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D211="","",IF(COUNTIF($D211:D397,D211)=1,D211,""))</f>
+        <v/>
+      </c>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="2"/>
+    </row>
+    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="E34" s="4"/>
       <c r="F34" s="1">
         <v>2</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="1" t="str">
-        <f>IF(D211="","",IF(COUNTIF($D211:D397,D211)=1,D211,""))</f>
-        <v/>
-      </c>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="2"/>
-    </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D212="","",IF(COUNTIF($D212:D398,D212)=1,D212,""))</f>
+        <v/>
+      </c>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="2"/>
+    </row>
+    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D35" s="1" t="s">
         <v>19</v>
       </c>
@@ -1581,20 +1754,20 @@
         <v>2</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.964</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="1" t="str">
-        <f>IF(D212="","",IF(COUNTIF($D212:D398,D212)=1,D212,""))</f>
-        <v/>
-      </c>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="2"/>
-    </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D213="","",IF(COUNTIF($D213:D399,D213)=1,D213,""))</f>
+        <v/>
+      </c>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="2"/>
+    </row>
+    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D36" s="1" t="s">
         <v>29</v>
       </c>
@@ -1605,40 +1778,40 @@
         <v>2</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="I36" s="2"/>
-      <c r="J36" s="1" t="str">
-        <f>IF(D213="","",IF(COUNTIF($D213:D399,D213)=1,D213,""))</f>
-        <v/>
-      </c>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="2"/>
-    </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J36" s="5" t="str">
+        <f>IF(A214="","",IF(COUNTIF($D214:D392,D214)=1,D214,""))</f>
+        <v/>
+      </c>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="2"/>
+    </row>
+    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="4"/>
       <c r="F37" s="1">
         <v>2</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="5" t="str">
-        <f>IF(A214="","",IF(COUNTIF($D214:D392,D214)=1,D214,""))</f>
-        <v/>
-      </c>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="2"/>
-    </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(A215="","",IF(COUNTIF($D215:D393,D215)=1,D215,""))</f>
+        <v/>
+      </c>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="2"/>
+    </row>
+    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>30</v>
       </c>
@@ -1648,40 +1821,40 @@
         <v>12</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="5" t="str">
-        <f>IF(A215="","",IF(COUNTIF($D215:D393,D215)=1,D215,""))</f>
-        <v/>
-      </c>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="2"/>
-    </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(A216="","",IF(COUNTIF($D216:D394,D216)=1,D216,""))</f>
+        <v/>
+      </c>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="2"/>
+    </row>
+    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D39" s="1"/>
       <c r="E39" s="4"/>
       <c r="F39" s="1">
         <v>12</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="5" t="str">
-        <f>IF(A216="","",IF(COUNTIF($D216:D394,D216)=1,D216,""))</f>
-        <v/>
-      </c>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="2"/>
-    </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(A217="","",IF(COUNTIF($D217:D395,D217)=1,D217,""))</f>
+        <v/>
+      </c>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="2"/>
+    </row>
+    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D40" s="1" t="s">
         <v>19</v>
       </c>
@@ -1692,40 +1865,40 @@
         <v>12</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="5" t="str">
-        <f>IF(A217="","",IF(COUNTIF($D217:D395,D217)=1,D217,""))</f>
-        <v/>
-      </c>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="2"/>
-    </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(A218="","",IF(COUNTIF($D218:D396,D218)=1,D218,""))</f>
+        <v/>
+      </c>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="2"/>
+    </row>
+    <row r="41" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D41" s="1"/>
       <c r="E41" s="4"/>
       <c r="F41" s="1">
         <v>12</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="5" t="str">
-        <f>IF(A218="","",IF(COUNTIF($D218:D396,D218)=1,D218,""))</f>
-        <v/>
-      </c>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="2"/>
-    </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(A219="","",IF(COUNTIF($D219:D397,D219)=1,D219,""))</f>
+        <v/>
+      </c>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="2"/>
+    </row>
+    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>31</v>
       </c>
@@ -1735,40 +1908,40 @@
         <v>38</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="5" t="str">
-        <f>IF(A219="","",IF(COUNTIF($D219:D397,D219)=1,D219,""))</f>
-        <v/>
-      </c>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="2"/>
-    </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(A220="","",IF(COUNTIF($D220:D398,D220)=1,D220,""))</f>
+        <v/>
+      </c>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="2"/>
+    </row>
+    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
       <c r="E43" s="4"/>
       <c r="F43" s="1">
         <v>38</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="5" t="str">
-        <f>IF(A220="","",IF(COUNTIF($D220:D398,D220)=1,D220,""))</f>
-        <v/>
-      </c>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="2"/>
-    </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(A221="","",IF(COUNTIF($D221:D399,D221)=1,D221,""))</f>
+        <v/>
+      </c>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="2"/>
+    </row>
+    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D44" s="1" t="s">
         <v>19</v>
       </c>
@@ -1779,20 +1952,20 @@
         <v>38</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>21.166</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="5" t="str">
-        <f>IF(A221="","",IF(COUNTIF($D221:D399,D221)=1,D221,""))</f>
-        <v/>
-      </c>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="2"/>
-    </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(A222="","",IF(COUNTIF($D222:D400,D222)=1,D222,""))</f>
+        <v/>
+      </c>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="2"/>
+    </row>
+    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D45" s="1" t="s">
         <v>32</v>
       </c>
@@ -1803,40 +1976,40 @@
         <v>38</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16.795999999999999</v>
       </c>
       <c r="I45" s="2"/>
-      <c r="J45" s="5" t="str">
-        <f>IF(A222="","",IF(COUNTIF($D222:D400,D222)=1,D222,""))</f>
-        <v/>
-      </c>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="2"/>
-    </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J45" s="1" t="str">
+        <f>IF(D223="","",IF(COUNTIF($D223:D409,D223)=1,D223,""))</f>
+        <v/>
+      </c>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="2"/>
+    </row>
+    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
       <c r="E46" s="4"/>
       <c r="F46" s="1">
         <v>38</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="1" t="str">
-        <f>IF(D223="","",IF(COUNTIF($D223:D409,D223)=1,D223,""))</f>
-        <v/>
-      </c>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="2"/>
-    </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D224="","",IF(COUNTIF($D224:D410,D224)=1,D224,""))</f>
+        <v/>
+      </c>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="2"/>
+    </row>
+    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>33</v>
       </c>
@@ -1846,40 +2019,40 @@
         <v>1</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="1" t="str">
-        <f>IF(D224="","",IF(COUNTIF($D224:D410,D224)=1,D224,""))</f>
-        <v/>
-      </c>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="2"/>
-    </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D225="","",IF(COUNTIF($D225:D411,D225)=1,D225,""))</f>
+        <v/>
+      </c>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="2"/>
+    </row>
+    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
       <c r="E48" s="4"/>
       <c r="F48" s="1">
         <v>1</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="1" t="str">
-        <f>IF(D225="","",IF(COUNTIF($D225:D411,D225)=1,D225,""))</f>
-        <v/>
-      </c>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="2"/>
-    </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D226="","",IF(COUNTIF($D226:D412,D226)=1,D226,""))</f>
+        <v/>
+      </c>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="2"/>
+    </row>
+    <row r="49" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D49" s="1" t="s">
         <v>19</v>
       </c>
@@ -1890,40 +2063,36 @@
         <v>1</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="1" t="str">
-        <f>IF(D226="","",IF(COUNTIF($D226:D412,D226)=1,D226,""))</f>
-        <v/>
-      </c>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="2"/>
-    </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+        <f>IF(D227="","",IF(COUNTIF($D227:D413,D227)=1,D227,""))</f>
+        <v/>
+      </c>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="2"/>
+    </row>
+    <row r="50" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
       <c r="E50" s="4"/>
       <c r="F50" s="1">
         <v>1</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I50" s="2"/>
-      <c r="J50" s="1" t="str">
-        <f>IF(D227="","",IF(COUNTIF($D227:D413,D227)=1,D227,""))</f>
-        <v/>
-      </c>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="2"/>
-    </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="2"/>
+    </row>
+    <row r="51" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>34</v>
       </c>
@@ -1933,32 +2102,32 @@
         <v>8</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I51" s="2"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="2"/>
-    </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="2"/>
+    </row>
+    <row r="52" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
       <c r="E52" s="4"/>
       <c r="F52" s="1">
         <v>8</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I52" s="2"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="2"/>
-    </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="2"/>
+    </row>
+    <row r="53" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D53" s="1" t="s">
         <v>19</v>
       </c>
@@ -1969,32 +2138,32 @@
         <v>8</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="I53" s="2"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="2"/>
-    </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="2"/>
+    </row>
+    <row r="54" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
       <c r="E54" s="4"/>
       <c r="F54" s="1">
         <v>8</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I54" s="2"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="2"/>
-    </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="2"/>
+    </row>
+    <row r="55" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>35</v>
       </c>
@@ -2004,32 +2173,32 @@
         <v>34</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I55" s="2"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="2"/>
-    </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="2"/>
+    </row>
+    <row r="56" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="E56" s="4"/>
       <c r="F56" s="1">
         <v>34</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I56" s="2"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="2"/>
-    </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="2"/>
+    </row>
+    <row r="57" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D57" s="1" t="s">
         <v>19</v>
       </c>
@@ -2040,32 +2209,32 @@
         <v>34</v>
       </c>
       <c r="H57" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="I57" s="2"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="2"/>
-    </row>
-    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="2"/>
+    </row>
+    <row r="58" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="E58" s="4"/>
       <c r="F58" s="1">
         <v>34</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I58" s="2"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="2"/>
-    </row>
-    <row r="59" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="2"/>
+    </row>
+    <row r="59" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>36</v>
       </c>
@@ -2075,32 +2244,32 @@
         <v>1</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I59" s="2"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="2"/>
-    </row>
-    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="2"/>
+    </row>
+    <row r="60" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D60" s="1"/>
       <c r="E60" s="4"/>
       <c r="F60" s="1">
         <v>1</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I60" s="2"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="2"/>
-    </row>
-    <row r="61" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="2"/>
+    </row>
+    <row r="61" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D61" s="1" t="s">
         <v>19</v>
       </c>
@@ -2111,32 +2280,32 @@
         <v>1</v>
       </c>
       <c r="H61" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I61" s="2"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="2"/>
-    </row>
-    <row r="62" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="2"/>
+    </row>
+    <row r="62" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D62" s="1"/>
       <c r="E62" s="4"/>
       <c r="F62" s="1">
         <v>1</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I62" s="2"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="2"/>
-    </row>
-    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="2"/>
+    </row>
+    <row r="63" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>37</v>
       </c>
@@ -2146,32 +2315,32 @@
         <v>3</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I63" s="2"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="2"/>
-    </row>
-    <row r="64" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="2"/>
+    </row>
+    <row r="64" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D64" s="1"/>
       <c r="E64" s="4"/>
       <c r="F64" s="1">
         <v>3</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I64" s="2"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="2"/>
-    </row>
-    <row r="65" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="2"/>
+    </row>
+    <row r="65" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D65" s="1" t="s">
         <v>19</v>
       </c>
@@ -2182,32 +2351,32 @@
         <v>3</v>
       </c>
       <c r="H65" s="1">
-        <f t="shared" ref="H65:H128" si="1">IF($E65*$F65=0,"",$E65*$F65)</f>
+        <f t="shared" ref="H65:H128" si="5">IF($E65*$F65=0,"",$E65*$F65)</f>
         <v>3</v>
       </c>
       <c r="I65" s="2"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="2"/>
-    </row>
-    <row r="66" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="2"/>
+    </row>
+    <row r="66" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D66" s="1"/>
       <c r="E66" s="4"/>
       <c r="F66" s="1">
         <v>3</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I66" s="2"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="2"/>
-    </row>
-    <row r="67" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="2"/>
+    </row>
+    <row r="67" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>38</v>
       </c>
@@ -2217,32 +2386,32 @@
         <v>11</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I67" s="2"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="2"/>
-    </row>
-    <row r="68" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="2"/>
+    </row>
+    <row r="68" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D68" s="1"/>
       <c r="E68" s="4"/>
       <c r="F68" s="1">
         <v>11</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I68" s="2"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="2"/>
-    </row>
-    <row r="69" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="2"/>
+    </row>
+    <row r="69" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D69" s="1" t="s">
         <v>19</v>
       </c>
@@ -2253,16 +2422,16 @@
         <v>11</v>
       </c>
       <c r="H69" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9.7460000000000004</v>
       </c>
       <c r="I69" s="2"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="2"/>
-    </row>
-    <row r="70" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="2"/>
+    </row>
+    <row r="70" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D70" s="1" t="s">
         <v>29</v>
       </c>
@@ -2273,32 +2442,32 @@
         <v>11</v>
       </c>
       <c r="H70" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.2430000000000001</v>
       </c>
       <c r="I70" s="2"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="2"/>
-    </row>
-    <row r="71" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="2"/>
+    </row>
+    <row r="71" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D71" s="1"/>
       <c r="E71" s="4"/>
       <c r="F71" s="1">
         <v>11</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I71" s="2"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="2"/>
-    </row>
-    <row r="72" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="2"/>
+    </row>
+    <row r="72" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>39</v>
       </c>
@@ -2308,32 +2477,32 @@
         <v>26</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I72" s="2"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="2"/>
-    </row>
-    <row r="73" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="2"/>
+    </row>
+    <row r="73" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D73" s="1"/>
       <c r="E73" s="4"/>
       <c r="F73" s="1">
         <v>26</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I73" s="2"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="2"/>
-    </row>
-    <row r="74" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="2"/>
+    </row>
+    <row r="74" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D74" s="1" t="s">
         <v>19</v>
       </c>
@@ -2344,32 +2513,32 @@
         <v>26</v>
       </c>
       <c r="H74" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="I74" s="2"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="2"/>
-    </row>
-    <row r="75" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="2"/>
+    </row>
+    <row r="75" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D75" s="1"/>
       <c r="E75" s="4"/>
       <c r="F75" s="1">
         <v>26</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I75" s="2"/>
-      <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="2"/>
-    </row>
-    <row r="76" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="2"/>
+    </row>
+    <row r="76" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
         <v>40</v>
       </c>
@@ -2379,32 +2548,32 @@
         <v>5</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I76" s="2"/>
-      <c r="L76" s="1"/>
-      <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
-      <c r="O76" s="2"/>
-    </row>
-    <row r="77" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="2"/>
+    </row>
+    <row r="77" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D77" s="1"/>
       <c r="E77" s="4"/>
       <c r="F77" s="1">
         <v>5</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I77" s="2"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="2"/>
-    </row>
-    <row r="78" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="2"/>
+    </row>
+    <row r="78" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D78" s="1" t="s">
         <v>19</v>
       </c>
@@ -2415,32 +2584,32 @@
         <v>5</v>
       </c>
       <c r="H78" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="I78" s="2"/>
-      <c r="L78" s="1"/>
-      <c r="M78" s="1"/>
-      <c r="N78" s="1"/>
-      <c r="O78" s="2"/>
-    </row>
-    <row r="79" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="2"/>
+    </row>
+    <row r="79" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D79" s="1"/>
       <c r="E79" s="4"/>
       <c r="F79" s="1">
         <v>5</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I79" s="2"/>
-      <c r="L79" s="1"/>
-      <c r="M79" s="1"/>
-      <c r="N79" s="1"/>
-      <c r="O79" s="2"/>
-    </row>
-    <row r="80" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="2"/>
+    </row>
+    <row r="80" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>41</v>
       </c>
@@ -2450,32 +2619,32 @@
         <v>8</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I80" s="2"/>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
-      <c r="N80" s="1"/>
-      <c r="O80" s="2"/>
-    </row>
-    <row r="81" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="2"/>
+    </row>
+    <row r="81" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D81" s="1"/>
       <c r="E81" s="4"/>
       <c r="F81" s="1">
         <v>8</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I81" s="2"/>
-      <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
-      <c r="N81" s="1"/>
-      <c r="O81" s="2"/>
-    </row>
-    <row r="82" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="2"/>
+    </row>
+    <row r="82" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D82" s="1" t="s">
         <v>19</v>
       </c>
@@ -2486,32 +2655,32 @@
         <v>8</v>
       </c>
       <c r="H82" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I82" s="2"/>
-      <c r="L82" s="1"/>
-      <c r="M82" s="1"/>
-      <c r="N82" s="1"/>
-      <c r="O82" s="2"/>
-    </row>
-    <row r="83" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="2"/>
+    </row>
+    <row r="83" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D83" s="1"/>
       <c r="E83" s="4"/>
       <c r="F83" s="1">
         <v>8</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I83" s="2"/>
-      <c r="L83" s="1"/>
-      <c r="M83" s="1"/>
-      <c r="N83" s="1"/>
-      <c r="O83" s="2"/>
-    </row>
-    <row r="84" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="2"/>
+    </row>
+    <row r="84" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>42</v>
       </c>
@@ -2521,32 +2690,32 @@
         <v>4</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I84" s="2"/>
-      <c r="L84" s="1"/>
-      <c r="M84" s="1"/>
-      <c r="N84" s="1"/>
-      <c r="O84" s="2"/>
-    </row>
-    <row r="85" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="2"/>
+    </row>
+    <row r="85" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D85" s="1"/>
       <c r="E85" s="4"/>
       <c r="F85" s="1">
         <v>4</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I85" s="2"/>
-      <c r="L85" s="1"/>
-      <c r="M85" s="1"/>
-      <c r="N85" s="1"/>
-      <c r="O85" s="2"/>
-    </row>
-    <row r="86" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="2"/>
+    </row>
+    <row r="86" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D86" s="1" t="s">
         <v>19</v>
       </c>
@@ -2557,16 +2726,16 @@
         <v>4</v>
       </c>
       <c r="H86" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.7480000000000002</v>
       </c>
       <c r="I86" s="2"/>
-      <c r="L86" s="1"/>
-      <c r="M86" s="1"/>
-      <c r="N86" s="1"/>
-      <c r="O86" s="2"/>
-    </row>
-    <row r="87" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="2"/>
+    </row>
+    <row r="87" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D87" s="1" t="s">
         <v>77</v>
       </c>
@@ -2577,16 +2746,16 @@
         <v>4</v>
       </c>
       <c r="H87" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.24</v>
       </c>
       <c r="I87" s="2"/>
-      <c r="L87" s="1"/>
-      <c r="M87" s="1"/>
-      <c r="N87" s="1"/>
-      <c r="O87" s="2"/>
-    </row>
-    <row r="88" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+      <c r="Q87" s="1"/>
+      <c r="R87" s="2"/>
+    </row>
+    <row r="88" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
         <v>43</v>
       </c>
@@ -2596,32 +2765,32 @@
         <v>22</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I88" s="2"/>
-      <c r="L88" s="1"/>
-      <c r="M88" s="1"/>
-      <c r="N88" s="1"/>
-      <c r="O88" s="2"/>
-    </row>
-    <row r="89" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+      <c r="Q88" s="1"/>
+      <c r="R88" s="2"/>
+    </row>
+    <row r="89" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D89" s="1"/>
       <c r="E89" s="4"/>
       <c r="F89" s="1">
         <v>22</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I89" s="2"/>
-      <c r="L89" s="1"/>
-      <c r="M89" s="1"/>
-      <c r="N89" s="1"/>
-      <c r="O89" s="2"/>
-    </row>
-    <row r="90" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
+      <c r="R89" s="2"/>
+    </row>
+    <row r="90" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D90" s="1" t="s">
         <v>19</v>
       </c>
@@ -2632,32 +2801,32 @@
         <v>22</v>
       </c>
       <c r="H90" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="I90" s="2"/>
-      <c r="L90" s="1"/>
-      <c r="M90" s="1"/>
-      <c r="N90" s="1"/>
-      <c r="O90" s="2"/>
-    </row>
-    <row r="91" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="2"/>
+    </row>
+    <row r="91" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D91" s="1"/>
       <c r="E91" s="4"/>
       <c r="F91" s="1">
         <v>22</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I91" s="2"/>
-      <c r="L91" s="1"/>
-      <c r="M91" s="1"/>
-      <c r="N91" s="1"/>
-      <c r="O91" s="2"/>
-    </row>
-    <row r="92" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="2"/>
+    </row>
+    <row r="92" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
         <v>44</v>
       </c>
@@ -2667,32 +2836,32 @@
         <v>0</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I92" s="2"/>
-      <c r="L92" s="1"/>
-      <c r="M92" s="1"/>
-      <c r="N92" s="1"/>
-      <c r="O92" s="2"/>
-    </row>
-    <row r="93" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="2"/>
+    </row>
+    <row r="93" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D93" s="1"/>
       <c r="E93" s="4"/>
       <c r="F93" s="1">
         <v>0</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I93" s="2"/>
-      <c r="L93" s="1"/>
-      <c r="M93" s="1"/>
-      <c r="N93" s="1"/>
-      <c r="O93" s="2"/>
-    </row>
-    <row r="94" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O93" s="1"/>
+      <c r="P93" s="1"/>
+      <c r="Q93" s="1"/>
+      <c r="R93" s="2"/>
+    </row>
+    <row r="94" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
         <v>45</v>
       </c>
@@ -2702,32 +2871,32 @@
         <v>3</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I94" s="2"/>
-      <c r="L94" s="1"/>
-      <c r="M94" s="1"/>
-      <c r="N94" s="1"/>
-      <c r="O94" s="2"/>
-    </row>
-    <row r="95" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="2"/>
+    </row>
+    <row r="95" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D95" s="1"/>
       <c r="E95" s="4"/>
       <c r="F95" s="1">
         <v>3</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I95" s="2"/>
-      <c r="L95" s="1"/>
-      <c r="M95" s="1"/>
-      <c r="N95" s="1"/>
-      <c r="O95" s="2"/>
-    </row>
-    <row r="96" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="2"/>
+    </row>
+    <row r="96" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D96" s="1" t="s">
         <v>19</v>
       </c>
@@ -2738,16 +2907,16 @@
         <v>3</v>
       </c>
       <c r="H96" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2.7510000000000003</v>
       </c>
       <c r="I96" s="2"/>
-      <c r="L96" s="1"/>
-      <c r="M96" s="1"/>
-      <c r="N96" s="1"/>
-      <c r="O96" s="2"/>
-    </row>
-    <row r="97" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="2"/>
+    </row>
+    <row r="97" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D97" s="1" t="s">
         <v>32</v>
       </c>
@@ -2758,32 +2927,32 @@
         <v>3</v>
       </c>
       <c r="H97" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.246</v>
       </c>
       <c r="I97" s="2"/>
-      <c r="L97" s="1"/>
-      <c r="M97" s="1"/>
-      <c r="N97" s="1"/>
-      <c r="O97" s="2"/>
-    </row>
-    <row r="98" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1"/>
+      <c r="R97" s="2"/>
+    </row>
+    <row r="98" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D98" s="1"/>
       <c r="E98" s="4"/>
       <c r="F98" s="1">
         <v>3</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I98" s="2"/>
-      <c r="L98" s="1"/>
-      <c r="M98" s="1"/>
-      <c r="N98" s="1"/>
-      <c r="O98" s="2"/>
-    </row>
-    <row r="99" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1"/>
+      <c r="R98" s="2"/>
+    </row>
+    <row r="99" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
         <v>46</v>
       </c>
@@ -2793,32 +2962,32 @@
         <v>7</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I99" s="2"/>
-      <c r="L99" s="1"/>
-      <c r="M99" s="1"/>
-      <c r="N99" s="1"/>
-      <c r="O99" s="2"/>
-    </row>
-    <row r="100" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O99" s="1"/>
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1"/>
+      <c r="R99" s="2"/>
+    </row>
+    <row r="100" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D100" s="1"/>
       <c r="E100" s="4"/>
       <c r="F100" s="1">
         <v>7</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I100" s="2"/>
-      <c r="L100" s="1"/>
-      <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
-      <c r="O100" s="2"/>
-    </row>
-    <row r="101" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="2"/>
+    </row>
+    <row r="101" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D101" s="1" t="s">
         <v>19</v>
       </c>
@@ -2829,32 +2998,32 @@
         <v>7</v>
       </c>
       <c r="H101" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="I101" s="2"/>
-      <c r="L101" s="1"/>
-      <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
-      <c r="O101" s="2"/>
-    </row>
-    <row r="102" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="2"/>
+    </row>
+    <row r="102" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D102" s="1"/>
       <c r="E102" s="4"/>
       <c r="F102" s="1">
         <v>7</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I102" s="2"/>
-      <c r="L102" s="1"/>
-      <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
-      <c r="O102" s="2"/>
-    </row>
-    <row r="103" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="2"/>
+    </row>
+    <row r="103" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C103" t="s">
         <v>47</v>
       </c>
@@ -2864,32 +3033,32 @@
         <v>11</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I103" s="2"/>
-      <c r="L103" s="1"/>
-      <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
-      <c r="O103" s="2"/>
-    </row>
-    <row r="104" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O103" s="1"/>
+      <c r="P103" s="1"/>
+      <c r="Q103" s="1"/>
+      <c r="R103" s="2"/>
+    </row>
+    <row r="104" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D104" s="1"/>
       <c r="E104" s="4"/>
       <c r="F104" s="1">
         <v>11</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I104" s="2"/>
-      <c r="L104" s="1"/>
-      <c r="M104" s="1"/>
-      <c r="N104" s="1"/>
-      <c r="O104" s="2"/>
-    </row>
-    <row r="105" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O104" s="1"/>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="1"/>
+      <c r="R104" s="2"/>
+    </row>
+    <row r="105" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D105" s="1" t="s">
         <v>19</v>
       </c>
@@ -2900,32 +3069,32 @@
         <v>11</v>
       </c>
       <c r="H105" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="I105" s="2"/>
-      <c r="L105" s="1"/>
-      <c r="M105" s="1"/>
-      <c r="N105" s="1"/>
-      <c r="O105" s="2"/>
-    </row>
-    <row r="106" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O105" s="1"/>
+      <c r="P105" s="1"/>
+      <c r="Q105" s="1"/>
+      <c r="R105" s="2"/>
+    </row>
+    <row r="106" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D106" s="1"/>
       <c r="E106" s="4"/>
       <c r="F106" s="1">
         <v>11</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I106" s="2"/>
-      <c r="L106" s="1"/>
-      <c r="M106" s="1"/>
-      <c r="N106" s="1"/>
-      <c r="O106" s="2"/>
-    </row>
-    <row r="107" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O106" s="1"/>
+      <c r="P106" s="1"/>
+      <c r="Q106" s="1"/>
+      <c r="R106" s="2"/>
+    </row>
+    <row r="107" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
         <v>48</v>
       </c>
@@ -2935,32 +3104,32 @@
         <v>8</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I107" s="2"/>
-      <c r="L107" s="1"/>
-      <c r="M107" s="1"/>
-      <c r="N107" s="1"/>
       <c r="O107" s="1"/>
-    </row>
-    <row r="108" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P107" s="1"/>
+      <c r="Q107" s="1"/>
+      <c r="R107" s="1"/>
+    </row>
+    <row r="108" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D108" s="1"/>
       <c r="E108" s="4"/>
       <c r="F108" s="1">
         <v>8</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I108" s="2"/>
-      <c r="L108" s="1"/>
-      <c r="M108" s="1"/>
-      <c r="N108" s="1"/>
       <c r="O108" s="1"/>
-    </row>
-    <row r="109" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P108" s="1"/>
+      <c r="Q108" s="1"/>
+      <c r="R108" s="1"/>
+    </row>
+    <row r="109" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D109" s="1" t="s">
         <v>19</v>
       </c>
@@ -2971,32 +3140,32 @@
         <v>8</v>
       </c>
       <c r="H109" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I109" s="2"/>
-      <c r="L109" s="1"/>
-      <c r="M109" s="1"/>
-      <c r="N109" s="1"/>
       <c r="O109" s="1"/>
-    </row>
-    <row r="110" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P109" s="1"/>
+      <c r="Q109" s="1"/>
+      <c r="R109" s="1"/>
+    </row>
+    <row r="110" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D110" s="1"/>
       <c r="E110" s="4"/>
       <c r="F110" s="1">
         <v>8</v>
       </c>
       <c r="H110" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I110" s="2"/>
-      <c r="L110" s="1"/>
-      <c r="M110" s="1"/>
-      <c r="N110" s="1"/>
       <c r="O110" s="1"/>
-    </row>
-    <row r="111" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P110" s="1"/>
+      <c r="Q110" s="1"/>
+      <c r="R110" s="1"/>
+    </row>
+    <row r="111" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C111" t="s">
         <v>49</v>
       </c>
@@ -3006,30 +3175,30 @@
         <v>6</v>
       </c>
       <c r="H111" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I111" s="2"/>
-      <c r="L111" s="1"/>
-      <c r="M111" s="1"/>
-      <c r="N111" s="1"/>
       <c r="O111" s="1"/>
-    </row>
-    <row r="112" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P111" s="1"/>
+      <c r="Q111" s="1"/>
+      <c r="R111" s="1"/>
+    </row>
+    <row r="112" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D112" s="1"/>
       <c r="E112" s="4"/>
       <c r="F112" s="1">
         <v>6</v>
       </c>
       <c r="H112" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I112" s="2"/>
-      <c r="L112" s="1"/>
-      <c r="M112" s="1"/>
-      <c r="N112" s="1"/>
       <c r="O112" s="1"/>
+      <c r="P112" s="1"/>
+      <c r="Q112" s="1"/>
+      <c r="R112" s="1"/>
     </row>
     <row r="113" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D113" s="1" t="s">
@@ -3042,7 +3211,7 @@
         <v>6</v>
       </c>
       <c r="H113" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="I113" s="2"/>
@@ -3054,7 +3223,7 @@
         <v>6</v>
       </c>
       <c r="H114" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I114" s="2"/>
@@ -3069,7 +3238,7 @@
         <v>7</v>
       </c>
       <c r="H115" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I115" s="2"/>
@@ -3081,7 +3250,7 @@
         <v>7</v>
       </c>
       <c r="H116" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I116" s="2"/>
@@ -3097,7 +3266,7 @@
         <v>7</v>
       </c>
       <c r="H117" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6.02</v>
       </c>
       <c r="I117" s="2"/>
@@ -3113,7 +3282,7 @@
         <v>7</v>
       </c>
       <c r="H118" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.97300000000000009</v>
       </c>
       <c r="I118" s="2"/>
@@ -3125,7 +3294,7 @@
         <v>7</v>
       </c>
       <c r="H119" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I119" s="2"/>
@@ -3140,7 +3309,7 @@
         <v>85</v>
       </c>
       <c r="H120" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I120" s="2"/>
@@ -3152,7 +3321,7 @@
         <v>85</v>
       </c>
       <c r="H121" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I121" s="2"/>
@@ -3168,7 +3337,7 @@
         <v>85</v>
       </c>
       <c r="H122" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>85</v>
       </c>
       <c r="I122" s="2"/>
@@ -3180,7 +3349,7 @@
         <v>85</v>
       </c>
       <c r="H123" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I123" s="2"/>
@@ -3195,7 +3364,7 @@
         <v>10</v>
       </c>
       <c r="H124" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I124" s="2"/>
@@ -3207,7 +3376,7 @@
         <v>10</v>
       </c>
       <c r="H125" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I125" s="2"/>
@@ -3223,7 +3392,7 @@
         <v>10</v>
       </c>
       <c r="H126" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="I126" s="2"/>
@@ -3235,7 +3404,7 @@
         <v>10</v>
       </c>
       <c r="H127" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I127" s="2"/>
@@ -3250,7 +3419,7 @@
         <v>0</v>
       </c>
       <c r="H128" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I128" s="2"/>
@@ -3262,7 +3431,7 @@
         <v>0</v>
       </c>
       <c r="H129" s="1" t="str">
-        <f t="shared" ref="H129:H164" si="2">IF($E129*$F129=0,"",$E129*$F129)</f>
+        <f t="shared" ref="H129:H164" si="6">IF($E129*$F129=0,"",$E129*$F129)</f>
         <v/>
       </c>
       <c r="I129" s="2"/>
@@ -3277,7 +3446,7 @@
         <v>4</v>
       </c>
       <c r="H130" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I130" s="2"/>
@@ -3289,7 +3458,7 @@
         <v>4</v>
       </c>
       <c r="H131" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I131" s="2"/>
@@ -3305,7 +3474,7 @@
         <v>4</v>
       </c>
       <c r="H132" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
       <c r="I132" s="2"/>
@@ -3321,7 +3490,7 @@
         <v>4</v>
       </c>
       <c r="H133" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.152</v>
       </c>
       <c r="I133" s="2"/>
@@ -3336,7 +3505,7 @@
         <v>0</v>
       </c>
       <c r="H134" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I134" s="2"/>
@@ -3350,8 +3519,12 @@
       <c r="F135" s="1">
         <v>4</v>
       </c>
+      <c r="G135" s="4">
+        <f>SUMPRODUCT(SUMIF($D$135:$D$157,J2,$H$135:$H$157))/K2</f>
+        <v>0</v>
+      </c>
       <c r="H135" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I135" s="2"/>
@@ -3363,8 +3536,12 @@
       <c r="F136" s="1">
         <v>4</v>
       </c>
+      <c r="G136" s="4">
+        <f t="shared" ref="G136:G138" si="7">SUMPRODUCT(SUMIF($D$135:$D$157,J3,$H$135:$H$157))/K3</f>
+        <v>2.8753632713418707E-2</v>
+      </c>
       <c r="H136" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I136" s="2"/>
@@ -3380,8 +3557,12 @@
       <c r="F137" s="1">
         <v>4</v>
       </c>
+      <c r="G137" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="H137" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="I137" s="2"/>
@@ -3393,8 +3574,12 @@
       <c r="F138" s="1">
         <v>4</v>
       </c>
+      <c r="G138" s="4">
+        <f t="shared" si="7"/>
+        <v>0.11975330818513862</v>
+      </c>
       <c r="H138" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I138" s="2"/>
@@ -3409,7 +3594,7 @@
         <v>4</v>
       </c>
       <c r="H139" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I139" s="2"/>
@@ -3422,7 +3607,7 @@
         <v>4</v>
       </c>
       <c r="H140" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I140" s="2"/>
@@ -3439,7 +3624,7 @@
         <v>4</v>
       </c>
       <c r="H141" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="I141" s="2"/>
@@ -3452,7 +3637,7 @@
         <v>4</v>
       </c>
       <c r="H142" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I142" s="2"/>
@@ -3467,7 +3652,7 @@
         <v>1</v>
       </c>
       <c r="H143" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I143" s="2"/>
@@ -3480,7 +3665,7 @@
         <v>1</v>
       </c>
       <c r="H144" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I144" s="2"/>
@@ -3497,7 +3682,7 @@
         <v>1</v>
       </c>
       <c r="H145" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I145" s="2"/>
@@ -3510,7 +3695,7 @@
         <v>1</v>
       </c>
       <c r="H146" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I146" s="2"/>
@@ -3525,7 +3710,7 @@
         <v>3</v>
       </c>
       <c r="H147" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I147" s="2"/>
@@ -3538,7 +3723,7 @@
         <v>3</v>
       </c>
       <c r="H148" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I148" s="2"/>
@@ -3555,7 +3740,7 @@
         <v>3</v>
       </c>
       <c r="H149" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I149" s="2"/>
@@ -3568,7 +3753,7 @@
         <v>3</v>
       </c>
       <c r="H150" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I150" s="2"/>
@@ -3583,7 +3768,7 @@
         <v>1</v>
       </c>
       <c r="H151" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I151" s="2"/>
@@ -3596,7 +3781,7 @@
         <v>1</v>
       </c>
       <c r="H152" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I152" s="2"/>
@@ -3613,7 +3798,7 @@
         <v>1</v>
       </c>
       <c r="H153" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I153" s="2"/>
@@ -3626,7 +3811,7 @@
         <v>1</v>
       </c>
       <c r="H154" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I154" s="2"/>
@@ -3641,7 +3826,7 @@
         <v>5</v>
       </c>
       <c r="H155" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I155" s="2"/>
@@ -3654,7 +3839,7 @@
         <v>5</v>
       </c>
       <c r="H156" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I156" s="2"/>
@@ -3671,7 +3856,7 @@
         <v>5</v>
       </c>
       <c r="H157" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="I157" s="2"/>
@@ -3688,8 +3873,12 @@
       <c r="F158" s="1">
         <v>0</v>
       </c>
+      <c r="G158" s="4">
+        <f>SUMPRODUCT(SUMIF($D$158:$D$184,J2,$H$158:$H$184))/K2</f>
+        <v>0</v>
+      </c>
       <c r="H158" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I158" s="2"/>
@@ -3701,8 +3890,12 @@
       <c r="F159" s="1">
         <v>0</v>
       </c>
+      <c r="G159" s="4">
+        <f t="shared" ref="G159:G161" si="8">SUMPRODUCT(SUMIF($D$158:$D$184,J3,$H$158:$H$184))/K3</f>
+        <v>0</v>
+      </c>
       <c r="H159" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I159" s="2"/>
@@ -3716,8 +3909,12 @@
       <c r="F160" s="1">
         <v>15</v>
       </c>
+      <c r="G160" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
       <c r="H160" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I160" s="2"/>
@@ -3729,8 +3926,12 @@
       <c r="F161" s="1">
         <v>15</v>
       </c>
+      <c r="G161" s="4">
+        <f t="shared" si="8"/>
+        <v>0.80833483024968567</v>
+      </c>
       <c r="H161" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I161" s="2"/>
@@ -3743,7 +3944,7 @@
         <v>15</v>
       </c>
       <c r="H162" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I162" s="2"/>
@@ -3760,7 +3961,7 @@
         <v>15</v>
       </c>
       <c r="H163" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="I163" s="2"/>
@@ -3775,7 +3976,7 @@
         <v>0</v>
       </c>
       <c r="H164" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I164" s="2"/>
@@ -3803,7 +4004,7 @@
         <v>0</v>
       </c>
       <c r="H166" s="1" t="str">
-        <f t="shared" ref="H166:H184" si="3">IFERROR(IF($E166*$F166=0,"",$E166*$F166),"")</f>
+        <f t="shared" ref="H166:H184" si="9">IFERROR(IF($E166*$F166=0,"",$E166*$F166),"")</f>
         <v/>
       </c>
       <c r="I166" s="2"/>
@@ -3816,7 +4017,7 @@
         <v>78</v>
       </c>
       <c r="H167" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I167" s="2"/>
@@ -3831,7 +4032,7 @@
         <v>0</v>
       </c>
       <c r="H168" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I168" s="2"/>
@@ -3844,7 +4045,7 @@
         <v>78</v>
       </c>
       <c r="H169" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I169" s="2"/>
@@ -3859,7 +4060,7 @@
         <v>0</v>
       </c>
       <c r="H170" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I170" s="2"/>
@@ -3872,7 +4073,7 @@
         <v>78</v>
       </c>
       <c r="H171" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I171" s="2"/>
@@ -3887,7 +4088,7 @@
         <v>0</v>
       </c>
       <c r="H172" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I172" s="2"/>
@@ -3900,7 +4101,7 @@
         <v>78</v>
       </c>
       <c r="H173" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I173" s="2"/>
@@ -3915,7 +4116,7 @@
         <v>0</v>
       </c>
       <c r="H174" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I174" s="2"/>
@@ -3928,7 +4129,7 @@
         <v>78</v>
       </c>
       <c r="H175" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I175" s="2"/>
@@ -3943,7 +4144,7 @@
         <v>15</v>
       </c>
       <c r="H176" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I176" s="2"/>
@@ -3956,7 +4157,7 @@
         <v>15</v>
       </c>
       <c r="H177" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I177" s="2"/>
@@ -3969,7 +4170,7 @@
         <v>15</v>
       </c>
       <c r="H178" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I178" s="2"/>
@@ -3986,7 +4187,7 @@
         <v>15</v>
       </c>
       <c r="H179" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="I179" s="2"/>
@@ -4001,7 +4202,7 @@
         <v>12</v>
       </c>
       <c r="H180" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I180" s="2"/>
@@ -4014,7 +4215,7 @@
         <v>12</v>
       </c>
       <c r="H181" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I181" s="2"/>
@@ -4027,7 +4228,7 @@
         <v>12</v>
       </c>
       <c r="H182" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I182" s="2"/>
@@ -4043,7 +4244,7 @@
         <v>12</v>
       </c>
       <c r="H183" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="I183" s="2"/>
@@ -4054,7 +4255,7 @@
         <v>12</v>
       </c>
       <c r="H184" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I184" s="2"/>
@@ -7356,16 +7557,12 @@
       <c r="I1282" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="J2:J29">
-    <sortState ref="J3:N232">
-      <sortCondition ref="J2:J211"/>
-    </sortState>
-  </autoFilter>
   <sortState ref="J2:J214">
     <sortCondition ref="J2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>